<commit_message>
Atualizações das minhas tarefas
</commit_message>
<xml_diff>
--- a/docs/drive/Tarefa S-01 Vitor.xlsx
+++ b/docs/drive/Tarefa S-01 Vitor.xlsx
@@ -1,26 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vitor\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F509CB-1FC5-40BB-A1E7-79700E29180E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="Página1" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Página1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="86">
   <si>
     <t>Quesitos / Modelo</t>
   </si>
@@ -118,61 +109,52 @@
     <t>24 GB</t>
   </si>
   <si>
-    <t>12–16 GB</t>
+    <t>35 GB</t>
+  </si>
+  <si>
+    <t>6 GB</t>
+  </si>
+  <si>
+    <t>400 GB</t>
+  </si>
+  <si>
+    <t>20 GB</t>
+  </si>
+  <si>
+    <t>240 GB</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>8 - 16 GB</t>
+  </si>
+  <si>
+    <t>64 GB</t>
+  </si>
+  <si>
+    <t>32 GB</t>
+  </si>
+  <si>
+    <t>128 GB</t>
   </si>
   <si>
     <t>160 GB</t>
   </si>
   <si>
-    <t>20 GB</t>
-  </si>
-  <si>
-    <t>96 GB</t>
-  </si>
-  <si>
-    <t>RAM</t>
-  </si>
-  <si>
-    <t>8 - 16 GB</t>
-  </si>
-  <si>
-    <t>64 GB</t>
-  </si>
-  <si>
-    <t>12 GB</t>
-  </si>
-  <si>
-    <t>14 GB</t>
-  </si>
-  <si>
-    <t>128 GB</t>
-  </si>
-  <si>
-    <t>32 - 64 GB</t>
-  </si>
-  <si>
-    <t>128 - 256 GB</t>
-  </si>
-  <si>
     <t>Armazenamento</t>
   </si>
   <si>
-    <t>100 GB SSD</t>
-  </si>
-  <si>
-    <t>500 GB SSD</t>
-  </si>
-  <si>
-    <t>40 GB</t>
-  </si>
-  <si>
-    <t>1 TB SSD</t>
-  </si>
-  <si>
-    <t>32 GB</t>
-  </si>
-  <si>
-    <t>100 - 200 GB</t>
+    <t>100 GB</t>
+  </si>
+  <si>
+    <t>500 GB</t>
+  </si>
+  <si>
+    <t>200 GB</t>
+  </si>
+  <si>
+    <t>300 GB</t>
   </si>
   <si>
     <t>Componente</t>
@@ -181,16 +163,16 @@
     <t>CPU cores</t>
   </si>
   <si>
-    <t>16–32</t>
+    <t>32-64</t>
+  </si>
+  <si>
+    <t>6 - 8</t>
   </si>
   <si>
     <t>32+</t>
   </si>
   <si>
-    <t>6 - 8</t>
-  </si>
-  <si>
-    <t>16 - 24</t>
+    <t>16 - 32</t>
   </si>
   <si>
     <t>CPU modelo</t>
@@ -199,7 +181,7 @@
     <t>Intel i5 / Ryzen 3 +</t>
   </si>
   <si>
-    <t>Intel i7/i9, Ryzen 9,  server-grade Xeon</t>
+    <t>AMD Threadripper PRO 5975WX</t>
   </si>
   <si>
     <t>Intel Core i7, Intel Xeon</t>
@@ -208,13 +190,10 @@
     <t>Intel i7-11800H</t>
   </si>
   <si>
-    <t>server-grade Xeon</t>
-  </si>
-  <si>
     <t>Intel Core i7 +</t>
   </si>
   <si>
-    <t>AMD Ryzen 9 7950X - Intel Core i9-13900K</t>
+    <t>Threadripper PRO 5975WX, Xeon 6338</t>
   </si>
   <si>
     <t>GPU</t>
@@ -229,16 +208,16 @@
     <t>NVIDIA RTX 4090</t>
   </si>
   <si>
-    <t>NVIDIA RTX 3060 12GB</t>
-  </si>
-  <si>
-    <t>2× NVIDIA A100 80GB</t>
-  </si>
-  <si>
-    <t>4× RTX 4090 GPUs</t>
-  </si>
-  <si>
-    <t>DDR4 ou DDR5</t>
+    <t>NVIDIA GTX 1660</t>
+  </si>
+  <si>
+    <t>4 × NVIDIA RTX 4090</t>
+  </si>
+  <si>
+    <t>NVIDIA RTX 3080 20GB</t>
+  </si>
+  <si>
+    <t>3x NVIDIA A100 80GB</t>
   </si>
   <si>
     <t>a</t>
@@ -253,6 +232,9 @@
     <t>Falcon</t>
   </si>
   <si>
+    <t>DeepSeek</t>
+  </si>
+  <si>
     <t>GPU System Requirements Guide for Gemma 3 Multimodal</t>
   </si>
   <si>
@@ -262,63 +244,107 @@
     <t>Blog - Guide to GPU Requirements for Running AI Models</t>
   </si>
   <si>
+    <t>Yi LLM: All Versions &amp; Hardware Requirements</t>
+  </si>
+  <si>
+    <t>A Step-by-Step Guide to Install DeepSeek-V3-0324 Locally - DEV Community</t>
+  </si>
+  <si>
+    <t>Running Gemma 3 Locally: A Step-by-Step Guide - DEV Community</t>
+  </si>
+  <si>
+    <t>Conquering LLaMA 3.3 70B VRAM Requirements for Home Servers</t>
+  </si>
+  <si>
+    <t>Falcon LLM: All Versions &amp; Hardware Requirements</t>
+  </si>
+  <si>
+    <t>How to Run Deepseek V3 0324 Locally (with Steps)</t>
+  </si>
+  <si>
     <t>Gemma 3: A Comprehensive Introduction</t>
   </si>
   <si>
     <t>Falcon 180B System Requirements &amp; Hardware Guide | Can You Run It?</t>
+  </si>
+  <si>
+    <t>DeepSeek Models System Requirements - Minimum and Recommended Hardware</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="14">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
-      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Roboto"/>
     </font>
     <font>
       <u/>
-      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Roboto"/>
     </font>
     <font>
       <u/>
-      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Roboto"/>
     </font>
     <font>
       <u/>
-      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Roboto"/>
     </font>
     <font>
       <u/>
-      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
       <color rgb="FF0000FF"/>
       <name val="Roboto"/>
     </font>
@@ -328,17 +354,11 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="24">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="21">
+    <border/>
     <border>
       <left style="thin">
         <color rgb="FF4A535C"/>
@@ -352,7 +372,6 @@
       <bottom style="thin">
         <color rgb="FF4A535C"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -367,7 +386,6 @@
       <bottom style="thin">
         <color rgb="FF4A535C"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -382,7 +400,6 @@
       <bottom style="thin">
         <color rgb="FF4A535C"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -397,7 +414,6 @@
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -412,7 +428,6 @@
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -427,7 +442,6 @@
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -442,7 +456,6 @@
       <bottom style="thin">
         <color rgb="FFF6F8F9"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -457,7 +470,6 @@
       <bottom style="thin">
         <color rgb="FFF6F8F9"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -472,7 +484,6 @@
       <bottom style="thin">
         <color rgb="FFF6F8F9"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -487,7 +498,6 @@
       <bottom style="thin">
         <color rgb="FF6AA84F"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -502,7 +512,6 @@
       <bottom style="thin">
         <color rgb="FFE69138"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -517,7 +526,6 @@
       <bottom style="thin">
         <color rgb="FF6AA84F"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -532,7 +540,6 @@
       <bottom style="thin">
         <color rgb="FFE69138"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -547,7 +554,6 @@
       <bottom style="thin">
         <color rgb="FFCC0000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -562,7 +568,6 @@
       <bottom style="thin">
         <color rgb="FFCC0000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -577,7 +582,6 @@
       <bottom style="thin">
         <color rgb="FF4A535C"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -592,7 +596,6 @@
       <bottom style="thin">
         <color rgb="FF4A535C"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -607,7 +610,6 @@
       <bottom style="thin">
         <color rgb="FF4A535C"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -622,7 +624,6 @@
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -637,486 +638,357 @@
       <bottom style="thin">
         <color rgb="FFF6F8F9"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF4A535C"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFF6F8F9"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFF6F8F9"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF4A535C"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFF6F8F9"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFF6F8F9"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFF6F8F9"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF4A535C"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFF6F8F9"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF4A535C"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFF6F8F9"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF4A535C"/>
-      </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="57">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="60">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="17" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="18" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="19" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="20" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="17" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="19" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="20" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="18" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="19" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="20" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="17" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="17" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="17" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="18" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="7">
     <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6AA84F"/>
+          <bgColor rgb="FF6AA84F"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCC0000"/>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFE69138"/>
           <bgColor rgb="FFE69138"/>
         </patternFill>
       </fill>
+      <border/>
     </dxf>
     <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
+          <fgColor rgb="FF626E7A"/>
+          <bgColor rgb="FF626E7A"/>
         </patternFill>
       </fill>
+      <border/>
     </dxf>
     <dxf>
+      <font/>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFE69138"/>
-          <bgColor rgb="FFE69138"/>
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
+      <border/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCC0000"/>
-          <bgColor rgb="FFCC0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
+      <font/>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFF6F8F9"/>
           <bgColor rgb="FFF6F8F9"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF356854"/>
-          <bgColor rgb="FF356854"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF6F8F9"/>
-          <bgColor rgb="FFF6F8F9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF626E7A"/>
-          <bgColor rgb="FF626E7A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF6F8F9"/>
-          <bgColor rgb="FFF6F8F9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF626E7A"/>
-          <bgColor rgb="FF626E7A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF6F8F9"/>
-          <bgColor rgb="FFF6F8F9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF626E7A"/>
-          <bgColor rgb="FF626E7A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF6F8F9"/>
-          <bgColor rgb="FFF6F8F9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF626E7A"/>
-          <bgColor rgb="FF626E7A"/>
-        </patternFill>
-      </fill>
+      <border/>
     </dxf>
   </dxfs>
-  <tableStyles count="5">
-    <tableStyle name="Página1-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="19"/>
-      <tableStyleElement type="firstRowStripe" dxfId="18"/>
-      <tableStyleElement type="secondRowStripe" dxfId="17"/>
+  <tableStyles count="4">
+    <tableStyle count="3" pivot="0" name="Página1-style">
+      <tableStyleElement dxfId="4" type="headerRow"/>
+      <tableStyleElement dxfId="5" type="firstRowStripe"/>
+      <tableStyleElement dxfId="6" type="secondRowStripe"/>
     </tableStyle>
-    <tableStyle name="Página1-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="headerRow" dxfId="16"/>
-      <tableStyleElement type="firstRowStripe" dxfId="15"/>
-      <tableStyleElement type="secondRowStripe" dxfId="14"/>
+    <tableStyle count="3" pivot="0" name="Página1-style 2">
+      <tableStyleElement dxfId="4" type="headerRow"/>
+      <tableStyleElement dxfId="5" type="firstRowStripe"/>
+      <tableStyleElement dxfId="6" type="secondRowStripe"/>
     </tableStyle>
-    <tableStyle name="Página1-style 3" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
-      <tableStyleElement type="headerRow" dxfId="13"/>
-      <tableStyleElement type="firstRowStripe" dxfId="12"/>
-      <tableStyleElement type="secondRowStripe" dxfId="11"/>
+    <tableStyle count="3" pivot="0" name="Página1-style 3">
+      <tableStyleElement dxfId="4" type="headerRow"/>
+      <tableStyleElement dxfId="5" type="firstRowStripe"/>
+      <tableStyleElement dxfId="6" type="secondRowStripe"/>
     </tableStyle>
-    <tableStyle name="Página1-style 4" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF03000000}">
-      <tableStyleElement type="headerRow" dxfId="10"/>
-      <tableStyleElement type="firstRowStripe" dxfId="9"/>
-      <tableStyleElement type="secondRowStripe" dxfId="8"/>
-    </tableStyle>
-    <tableStyle name="Página3-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF04000000}">
-      <tableStyleElement type="headerRow" dxfId="7"/>
-      <tableStyleElement type="firstRowStripe" dxfId="6"/>
-      <tableStyleElement type="secondRowStripe" dxfId="5"/>
+    <tableStyle count="3" pivot="0" name="Página1-style 4">
+      <tableStyleElement dxfId="4" type="headerRow"/>
+      <tableStyleElement dxfId="5" type="firstRowStripe"/>
+      <tableStyleElement dxfId="6" type="secondRowStripe"/>
     </tableStyle>
   </tableStyles>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Modelos_Diferentes" displayName="Modelos_Diferentes" ref="A1:H12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H12" displayName="Modelos_Diferentes" name="Modelos_Diferentes" id="1">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Quesitos / Modelo"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="GEMMA 3 1B"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="GEMMA 3 27B"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Llamma 3.3 70B"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Falcon 7B"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Falcon 180B"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Yi-34B"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="DeepSeek V3-0324"/>
+    <tableColumn name="Quesitos / Modelo" id="1"/>
+    <tableColumn name="GEMMA 3 1B" id="2"/>
+    <tableColumn name="GEMMA 3 27B" id="3"/>
+    <tableColumn name="Llamma 3.3 70B" id="4"/>
+    <tableColumn name="Falcon 7B" id="5"/>
+    <tableColumn name="Falcon 180B" id="6"/>
+    <tableColumn name="Yi-34B" id="7"/>
+    <tableColumn name="DeepSeek V3-0324" id="8"/>
   </tableColumns>
-  <tableStyleInfo name="Página1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="Página1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Hardwares_Mínimos" displayName="Hardwares_Mínimos" ref="A13:H16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A13:H16" displayName="Hardwares_Mínimos" name="Hardwares_Mínimos" id="2">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Harware Mínimo"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="GEMMA 3 1B"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="GEMMA 3 27B"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Llamma 3.3 70B"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Falcon 7B"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Falcon 180B"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Yi-34B (Quantizado - 4bit)"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="DeepSeek V3-0324 (Quantizado)"/>
+    <tableColumn name="Harware Mínimo" id="1"/>
+    <tableColumn name="GEMMA 3 1B" id="2"/>
+    <tableColumn name="GEMMA 3 27B" id="3"/>
+    <tableColumn name="Llamma 3.3 70B" id="4"/>
+    <tableColumn name="Falcon 7B" id="5"/>
+    <tableColumn name="Falcon 180B" id="6"/>
+    <tableColumn name="Yi-34B (Quantizado - 4bit)" id="7"/>
+    <tableColumn name="DeepSeek V3-0324 (Quantizado)" id="8"/>
   </tableColumns>
-  <tableStyleInfo name="Página1-style 2" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="Página1-style 2" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Recomendação_de_specs" displayName="Recomendação_de_specs" ref="A20:H24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A20:H23" displayName="Recomendação_de_specs" name="Recomendação_de_specs" id="3">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Componente"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="GEMMA 3 1B"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="GEMMA 3 27B"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Llamma 3.3 70B"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Falcon 7B"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Falcon 180B"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Yi-34B (Quantizado - 4bit)"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="DeepSeek V3-0324 (Quantizado)"/>
+    <tableColumn name="Componente" id="1"/>
+    <tableColumn name="GEMMA 3 1B" id="2"/>
+    <tableColumn name="GEMMA 3 27B" id="3"/>
+    <tableColumn name="Llamma 3.3 70B" id="4"/>
+    <tableColumn name="Falcon 7B" id="5"/>
+    <tableColumn name="Falcon 180B" id="6"/>
+    <tableColumn name="Yi-34B (Quantizado - 4bit)" id="7"/>
+    <tableColumn name="DeepSeek V3-0324 (Quantizado)" id="8"/>
   </tableColumns>
-  <tableStyleInfo name="Página1-style 3" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="Página1-style 3" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Referências" displayName="Referências" ref="A28:C30">
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="GEMMA 3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Llamma 3.3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Falcon"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A27:E30" displayName="Referências" name="Referências" id="4">
+  <tableColumns count="5">
+    <tableColumn name="GEMMA 3" id="1"/>
+    <tableColumn name="Llamma 3.3" id="2"/>
+    <tableColumn name="Falcon" id="3"/>
+    <tableColumn name="Yi-34B" id="4"/>
+    <tableColumn name="DeepSeek" id="5"/>
   </tableColumns>
-  <tableStyleInfo name="Página1-style 4" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="Página1-style 4" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1306,37 +1178,34 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.77734375" customWidth="1"/>
-    <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="23.44140625" customWidth="1"/>
-    <col min="8" max="8" width="29.6640625" customWidth="1"/>
-    <col min="9" max="9" width="14.77734375" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="29.38"/>
+    <col customWidth="1" min="2" max="2" width="15.38"/>
+    <col customWidth="1" min="3" max="3" width="19.13"/>
+    <col customWidth="1" min="4" max="4" width="17.63"/>
+    <col customWidth="1" min="5" max="5" width="19.75"/>
+    <col customWidth="1" min="6" max="6" width="19.0"/>
+    <col customWidth="1" min="7" max="7" width="23.5"/>
+    <col customWidth="1" min="8" max="8" width="29.63"/>
+    <col customWidth="1" min="9" max="9" width="14.75"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1362,21 +1231,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="7">
-        <v>2585</v>
+        <v>2585.0</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="8">
-        <v>276</v>
+        <v>276.0</v>
       </c>
       <c r="E2" s="8">
-        <v>100</v>
+        <v>100.0</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>9</v>
@@ -1388,33 +1257,33 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="12">
-        <v>32000</v>
+        <v>32000.0</v>
       </c>
       <c r="C3" s="12">
-        <v>128000</v>
+        <v>128000.0</v>
       </c>
       <c r="D3" s="12">
-        <v>128000</v>
+        <v>128000.0</v>
       </c>
       <c r="E3" s="12">
-        <v>2048</v>
+        <v>2048.0</v>
       </c>
       <c r="F3" s="12">
-        <v>4096</v>
+        <v>4096.0</v>
       </c>
       <c r="G3" s="13">
-        <v>200000</v>
+        <v>200000.0</v>
       </c>
       <c r="H3" s="14">
-        <v>32000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>32000.0</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" s="6" t="s">
         <v>13</v>
       </c>
@@ -1440,7 +1309,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" s="11" t="s">
         <v>16</v>
       </c>
@@ -1466,7 +1335,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" s="6" t="s">
         <v>17</v>
       </c>
@@ -1492,7 +1361,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" s="11" t="s">
         <v>18</v>
       </c>
@@ -1518,7 +1387,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8">
       <c r="A8" s="6" t="s">
         <v>21</v>
       </c>
@@ -1544,7 +1413,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="A9" s="11" t="s">
         <v>22</v>
       </c>
@@ -1570,7 +1439,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="A10" s="6" t="s">
         <v>23</v>
       </c>
@@ -1596,7 +1465,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="A11" s="24" t="s">
         <v>25</v>
       </c>
@@ -1622,7 +1491,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12">
       <c r="A12" s="25"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
@@ -1632,7 +1501,7 @@
       <c r="G12" s="26"/>
       <c r="H12" s="27"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13">
       <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
@@ -1658,7 +1527,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14">
       <c r="A14" s="28" t="s">
         <v>29</v>
       </c>
@@ -1669,83 +1538,79 @@
         <v>31</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F14" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="32" t="s">
         <v>33</v>
-      </c>
-      <c r="G14" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" s="30" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="32" t="s">
-        <v>40</v>
       </c>
       <c r="F15" s="32" t="s">
         <v>41</v>
       </c>
       <c r="G15" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="H15" s="33" t="s">
+    </row>
+    <row r="16">
+      <c r="A16" s="34" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
+      <c r="B16" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="35" t="s">
+      <c r="C16" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="D16" s="35" t="s">
         <v>46</v>
-      </c>
-      <c r="D16" s="35" t="s">
-        <v>47</v>
       </c>
       <c r="E16" s="35" t="s">
         <v>40</v>
       </c>
       <c r="F16" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" s="27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="C18" s="36"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="37" t="s">
         <v>48</v>
-      </c>
-      <c r="G16" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="H16" s="27" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C18" s="55"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="36" t="s">
-        <v>51</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>1</v>
@@ -1769,195 +1634,207 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="37" t="s">
+    <row r="21">
+      <c r="A21" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="8">
+        <v>16.0</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="9">
+        <v>8.0</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="8">
-        <v>16</v>
-      </c>
-      <c r="C21" s="8" t="s">
+      <c r="G21" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="H21" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="9">
-        <v>8</v>
-      </c>
-      <c r="E21" s="9">
-        <v>8</v>
-      </c>
-      <c r="F21" s="9" t="s">
+    </row>
+    <row r="22">
+      <c r="A22" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="B22" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="H21" s="10" t="s">
+      <c r="C22" s="32" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="38" t="s">
+      <c r="D22" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="32" t="s">
+      <c r="E22" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="32" t="s">
+      <c r="F22" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="32" t="s">
+      <c r="H22" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="E22" s="32" t="s">
+    </row>
+    <row r="23">
+      <c r="A23" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="F22" s="39" t="s">
+      <c r="B23" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="G22" s="32" t="s">
+      <c r="C23" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="H22" s="40" t="s">
+      <c r="D23" s="35" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="37" t="s">
+      <c r="E23" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="F23" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="G23" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="D23" s="29" t="s">
+      <c r="H23" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="E23" s="29" t="s">
+    </row>
+    <row r="24">
+      <c r="F24" s="43"/>
+      <c r="G24" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="F23" s="29" t="s">
+    </row>
+    <row r="25">
+      <c r="C25" s="43"/>
+    </row>
+    <row r="26">
+      <c r="E26" s="43"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="G23" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="H23" s="41" t="s">
+      <c r="B27" s="45" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="43" t="s">
+      <c r="C27" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="E24" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="F24" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="G24" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="H24" s="44" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F25" s="45"/>
-      <c r="G25" s="46" t="s">
+      <c r="D27" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C26" s="45"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E27" s="45"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="36" t="s">
+    <row r="28">
+      <c r="A28" s="46" t="s">
         <v>74</v>
       </c>
       <c r="B28" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="C28" s="48" t="s">
+      <c r="C28" s="47" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="49" t="s">
+      <c r="D28" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="B29" s="50" t="s">
+      <c r="E28" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="51" t="s">
+    </row>
+    <row r="29">
+      <c r="A29" s="50" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="52" t="s">
+      <c r="B29" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="B30" s="53"/>
-      <c r="C30" s="54" t="s">
+      <c r="C29" s="52" t="s">
         <v>81</v>
+      </c>
+      <c r="D29" s="53"/>
+      <c r="E29" s="54" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="55" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" s="56"/>
+      <c r="C30" s="57" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" s="58"/>
+      <c r="E30" s="59" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C18:G18"/>
   </mergeCells>
-  <conditionalFormatting sqref="B2:B20 C2:J18 K2:K13 C20:H20 C25:D25">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+  <conditionalFormatting sqref="B2:B20 C2:J18 K2:K13 C20:H20 C24:D24">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Sim"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B20 C2:J18 K2:K13 C20:H20 C25:D25">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+  <conditionalFormatting sqref="B2:B20 C2:J18 K2:K13 C20:H20 C24:D24">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Não"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B20 C2:J18 K2:K13 C20:H20 C25:D25">
+  <conditionalFormatting sqref="B2:B20 C2:J18 K2:K13 C20:H20 C24:D24">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Talvez"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:H7">
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"Bom"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:H7">
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>"Neutra"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A29" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B29" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C29" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="A30" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C30" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink r:id="rId1" ref="A28"/>
+    <hyperlink r:id="rId2" ref="B28"/>
+    <hyperlink r:id="rId3" ref="C28"/>
+    <hyperlink r:id="rId4" ref="D28"/>
+    <hyperlink r:id="rId5" ref="E28"/>
+    <hyperlink r:id="rId6" ref="A29"/>
+    <hyperlink r:id="rId7" ref="B29"/>
+    <hyperlink r:id="rId8" ref="C29"/>
+    <hyperlink r:id="rId9" ref="E29"/>
+    <hyperlink r:id="rId10" ref="A30"/>
+    <hyperlink r:id="rId11" ref="C30"/>
+    <hyperlink r:id="rId12" ref="E30"/>
   </hyperlinks>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId13"/>
   <tableParts count="4">
-    <tablePart r:id="rId6"/>
-    <tablePart r:id="rId7"/>
-    <tablePart r:id="rId8"/>
-    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId18"/>
+    <tablePart r:id="rId19"/>
+    <tablePart r:id="rId20"/>
+    <tablePart r:id="rId21"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>